<commit_message>
PIN-3458 Adjust list for livelihood - test resources adjustments
</commit_message>
<xml_diff>
--- a/tests/NewApiBundle/Resources/import-demo-3-country-specifics.xlsx
+++ b/tests/NewApiBundle/Resources/import-demo-3-country-specifics.xlsx
@@ -410,7 +410,7 @@
     <t xml:space="preserve">Thakurova</t>
   </si>
   <si>
-    <t xml:space="preserve">GoverNMEnt</t>
+    <t xml:space="preserve">Regular salary – PUBlic sector</t>
   </si>
   <si>
     <t xml:space="preserve">Poznamka cislo 1</t>
@@ -470,8 +470,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="D/M/YYYY"/>
-    <numFmt numFmtId="166" formatCode="DD\-MM\-YYYY"/>
+    <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="166" formatCode="dd\-mm\-yyyy"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -558,37 +558,34 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:BE6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O6" activeCellId="0" sqref="O6:Q6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="8.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="9.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="28" style="0" width="8.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="10.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="32" style="0" width="8.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="9.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="15.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="44" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1350,20 +1347,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="O6:Q6 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>